<commit_message>
Bar3D success but ugly.
</commit_message>
<xml_diff>
--- a/projectCities/data/radius_cities.xlsx
+++ b/projectCities/data/radius_cities.xlsx
@@ -436,17 +436,17 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>城市名</t>
+          <t>city_name</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>城市等级</t>
+          <t>city_level</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>通勤半径（千米）</t>
+          <t>radius</t>
         </is>
       </c>
     </row>

</xml_diff>